<commit_message>
Spike Refactor Plan update (GNkpakOQ)
</commit_message>
<xml_diff>
--- a/Resources/Spike Refactor Plan.xlsx
+++ b/Resources/Spike Refactor Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95A7AECB-2EA2-4DA1-8CAD-3F6B8005B664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00D75E1-E2CA-4C6C-BB7A-15F395658E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{9E6FF707-FC96-4033-B884-FBE91101AA82}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>}</t>
   </si>
@@ -192,44 +192,17 @@
     </r>
   </si>
   <si>
-    <t>┐</t>
-  </si>
-  <si>
-    <t>│</t>
-  </si>
-  <si>
-    <t>┘</t>
-  </si>
-  <si>
-    <r>
-      <t>│</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>this whole thing is in TrySpike on the AI and should be moved to the same</t>
-    </r>
+    <t>this whole thing is in TrySpike on the AI and should be moved to the same</t>
+  </si>
+  <si>
+    <t>transitions will be in the State that calls this method</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,13 +217,6 @@
       <family val="3"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Courier New"/>
@@ -302,23 +268,25 @@
       <family val="3"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF00B050"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color rgb="FF00B050"/>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF00B050"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -335,7 +303,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -343,11 +311,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFC000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFFC000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFFC000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFC000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFC000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFC000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFC000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFC000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFC000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFC000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -356,20 +417,46 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -707,25 +794,25 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="3" width="4.69140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="93.07421875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="1.69140625" style="4" customWidth="1"/>
-    <col min="6" max="8" width="4.69140625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="4.69140625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="58.3046875" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="9.23046875" style="4"/>
+    <col min="1" max="3" width="4.69140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="93.07421875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="1.69140625" style="3" customWidth="1"/>
+    <col min="6" max="8" width="4.69140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="4.69140625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="58.3046875" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="9.23046875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="23" t="s">
         <v>16</v>
       </c>
     </row>
@@ -759,10 +846,10 @@
       <c r="C6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -776,7 +863,7 @@
       <c r="I7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -791,11 +878,11 @@
       <c r="I8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
@@ -806,7 +893,7 @@
       <c r="I9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="K9" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -816,9 +903,8 @@
       <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>28</v>
-      </c>
+      <c r="E10" s="18"/>
+      <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="I10" s="1"/>
     </row>
@@ -828,9 +914,8 @@
       <c r="D11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>29</v>
-      </c>
+      <c r="E11" s="19"/>
+      <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="I11" s="1"/>
     </row>
@@ -840,8 +925,9 @@
       <c r="D12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>31</v>
+      <c r="E12" s="19"/>
+      <c r="F12" s="21" t="s">
+        <v>28</v>
       </c>
       <c r="G12" s="1"/>
       <c r="I12" s="1"/>
@@ -852,9 +938,8 @@
       <c r="D13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="9" t="s">
-        <v>29</v>
-      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="I13" s="1"/>
     </row>
@@ -864,21 +949,19 @@
       <c r="D14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>29</v>
-      </c>
+      <c r="E14" s="19"/>
+      <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="D15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="E15" s="20"/>
+      <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="I15" s="1"/>
     </row>
@@ -895,7 +978,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
@@ -907,7 +990,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="D18" s="2" t="s">
@@ -920,7 +1003,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
@@ -932,38 +1015,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1" t="s">
+      <c r="B20" s="8"/>
+      <c r="C20" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D20" s="10"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="I21" s="1" t="s">
+      <c r="B21" s="13"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="J21" s="17"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="8" t="s">
+      <c r="H22" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>0</v>
@@ -974,7 +1068,7 @@
       </c>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
@@ -984,19 +1078,20 @@
       <c r="G24" s="1"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.4">
       <c r="G27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Spike Refactor Plan update2 (GNkpakOQ)
</commit_message>
<xml_diff>
--- a/Resources/Spike Refactor Plan.xlsx
+++ b/Resources/Spike Refactor Plan.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00D75E1-E2CA-4C6C-BB7A-15F395658E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403AEDF1-128C-4D33-B7A5-254B6FB36075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{9E6FF707-FC96-4033-B884-FBE91101AA82}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Refactor" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>